<commit_message>
Bug fix for DB upgrade file (dependency issue)
</commit_message>
<xml_diff>
--- a/docs/Centralized Cruise Database - Business Rule List.xlsx
+++ b/docs/Centralized Cruise Database - Business Rule List.xlsx
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated application and phase 1 documentation with items that were completed or are planned
</commit_message>
<xml_diff>
--- a/docs/Centralized Cruise Database - Business Rule List.xlsx
+++ b/docs/Centralized Cruise Database - Business Rule List.xlsx
@@ -1043,16 +1043,16 @@
     <t>The "Inspect" link on the QC Validation Reports will forward the user to the View/Edit Cruise or Cruise Leg page based on which record needs to be inspected to resolve the given validation issue</t>
   </si>
   <si>
-    <t>Any authorized user that has the "DATA_ADMIN" role can add/edit/delete any records including user authorization records</t>
-  </si>
-  <si>
     <t>Data Admin Authorization</t>
   </si>
   <si>
     <t>Data Write Authorization</t>
   </si>
   <si>
-    <t>Any authorized user that has the "DATA_WRITE" role can add/edit/delete any cruise, cruise leg, and preset information as well as view/annotate validation issues</t>
+    <t>Any authorized user that has the "CCD ADMIN" role can add/edit/delete any records including user authorization records</t>
+  </si>
+  <si>
+    <t>Any authorized user that has the "CCD WRITE" role can add/edit/delete any cruise, cruise leg, and preset information as well as view/annotate validation issues</t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3126,10 +3126,10 @@
         <v>CR-DMA-004</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>14</v>
@@ -3648,7 +3648,7 @@
         <v>CR-DMA-019</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>240</v>

</xml_diff>

<commit_message>
fixed the Updated application to fix a bug with the standard survey name select list refresh process on page 220 and vessel list refresh process on page 230 Updated application URLs after disabling the APEX application alias (CCD)
</commit_message>
<xml_diff>
--- a/docs/Centralized Cruise Database - Business Rule List.xlsx
+++ b/docs/Centralized Cruise Database - Business Rule List.xlsx
@@ -1637,7 +1637,7 @@
   <dimension ref="A1:R372"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="D136" sqref="D136"/>
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6697,7 +6697,7 @@
         <v>134</v>
       </c>
       <c r="C148" s="9" t="str">
-        <f t="shared" ref="C148:C150" si="62">CONCATENATE("CR-DVM-ERR-", REPT("0", 3-LEN(A148)), A148)</f>
+        <f t="shared" ref="C148" si="62">CONCATENATE("CR-DVM-ERR-", REPT("0", 3-LEN(A148)), A148)</f>
         <v>CR-DVM-ERR-025</v>
       </c>
       <c r="D148" s="14" t="s">

</xml_diff>